<commit_message>
Update to Ginger.Plugin.Core 2.5.1
</commit_message>
<xml_diff>
--- a/GingerOfficePluginTest/TestResources/test1.xlsx
+++ b/GingerOfficePluginTest/TestResources/test1.xlsx
@@ -1,79 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15">
+  <x:fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <x:workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ginger\GingerNextVer_Dev\StandAloneActionsTest\TestResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9405" windowHeight="4920"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-  </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <x:bookViews>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="9405" windowHeight="4920"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+  </x:sheets>
+  <x:calcPr calcId="152511"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
-  <si>
-    <t>hello world</t>
-  </si>
-  <si>
-    <t>Dana</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>First</t>
-  </si>
-  <si>
-    <t>Last</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Used</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Cohen</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Moshe</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Roberts</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+  <x:si>
+    <x:t>hello world</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dana</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Smith</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>First</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Last</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Phone</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Used</x:t>
+  </x:si>
+  <x:si>
+    <x:t>David</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cohen</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Yes</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Moshe</x:t>
+  </x:si>
+  <x:si>
+    <x:t>No</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Roberts</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -427,93 +427,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2">
-        <v>923646</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>73769</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
-        <v>32</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2">
-        <v>878375</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:dimension ref="A1:E4"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection sqref="A1:XFD1"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="14" customWidth="1"/>
+    <x:col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <x:col min="3" max="4" width="12" customWidth="1"/>
+    <x:col min="5" max="5" width="13.5703125" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="1" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B1" s="1" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C1" s="1" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D1" s="1" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E1" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="2">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D2" s="2">
+        <x:v>923646</x:v>
+      </x:c>
+      <x:c r="E2" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="1">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B3" s="1" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C3" s="1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D3" s="1">
+        <x:v>73769</x:v>
+      </x:c>
+      <x:c r="E3" s="1" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="2">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="2">
+        <x:v>878375</x:v>
+      </x:c>
+      <x:c r="E4" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>